<commit_message>
now work for xls and xlsx with images sorted
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -5,18 +5,27 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\ecom_excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\imageFromExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97DAC2EE-BF99-440A-923F-6B037FAE809D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E162FC0F-4DCE-40A4-B59C-EC89D90209DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="765" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Quotation" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
@@ -143,7 +152,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="圖片 1">
+        <xdr:cNvPr id="2" name="圖片 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
@@ -186,7 +195,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="圖片 2">
+        <xdr:cNvPr id="3" name="圖片 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
@@ -217,19 +226,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>2081893</xdr:colOff>
+      <xdr:colOff>2095500</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>68036</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>707047</xdr:colOff>
+      <xdr:colOff>720654</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>154524</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="圖片 1">
+        <xdr:cNvPr id="6" name="圖片 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12C126E9-0A22-430B-A5E0-EC90304BE53E}"/>
@@ -248,7 +257,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9144000" y="3224893"/>
+          <a:off x="9157607" y="3224893"/>
           <a:ext cx="4190476" cy="4780952"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -260,20 +269,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>530678</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>598714</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>353785</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>194059</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>34786</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2180701</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>143642</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="圖片 3">
+        <xdr:cNvPr id="7" name="圖片 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D623577-3BF9-45DD-86B4-CA6404CD4946}"/>
@@ -292,8 +301,52 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14246678" y="3143250"/>
+          <a:off x="721178" y="9375321"/>
           <a:ext cx="4180952" cy="4742857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>326572</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>27215</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1128</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="圖片 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A09A9FAB-A363-4F41-9D90-08A5CD3AACEC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7388679" y="10327822"/>
+          <a:ext cx="5239878" cy="3034392"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -604,8 +657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V14" sqref="V14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>

</xml_diff>

<commit_message>
study on the bugs of handling multiple async call at the same time, fix minor part
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -13,9 +13,9 @@
   </bookViews>
   <sheets>
     <sheet name="Quotation" sheetId="1" r:id="rId1"/>
-    <sheet name="Images" sheetId="2" r:id="rId2"/>
+    <sheet name="Image" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,9 +34,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>DANIEL &amp; CO. - Quotation</t>
+  </si>
+  <si>
+    <t>Barcode</t>
   </si>
 </sst>
 </file>
@@ -358,6 +361,231 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>183375</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>653274</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Food, Health and Medicine: Majority of chemicals in ..."/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7727175" y="676276"/>
+          <a:ext cx="3213099" cy="2409825"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>411372</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>187085</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="Natural Hair Going Mainstream? | bellacoils"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1838325" y="657225"/>
+          <a:ext cx="3373647" cy="2530235"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>421500</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>174978</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>138793</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="圖片 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A09A9FAB-A363-4F41-9D90-08A5CD3AACEC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2478900" y="4905376"/>
+          <a:ext cx="5239878" cy="3034392"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>365124</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4" descr="Food, Health and Medicine: Majority of chemicals in ..."/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13611225" y="4438650"/>
+          <a:ext cx="3213099" cy="2409825"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>323327</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>142282</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="圖片 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D623577-3BF9-45DD-86B4-CA6404CD4946}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8486775" y="4800600"/>
+          <a:ext cx="4180952" cy="4742857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -657,7 +885,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X9"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
@@ -712,14 +940,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
-  <sheetData/>
+  <sheetData>
+    <row r="20" spans="8:8">
+      <c r="H20" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>